<commit_message>
Updated submission template file per PODCAT-855
</commit_message>
<xml_diff>
--- a/Public/Childhood_Cancer_Data_Catalog_Submission_Template.xlsx
+++ b/Public/Childhood_Cancer_Data_Catalog_Submission_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25721"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25924"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF574EF1-14DE-4A74-958B-E0327342A026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{1DBD8EDA-8D16-48B6-ABF1-40CB9C71B357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7A6E1AF-0EC4-4C7D-87EE-5B3B82C44EC2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="3" xr2:uid="{A813E664-7740-450B-B9AA-D361BEDD0A87}"/>
+    <workbookView xWindow="32892" yWindow="792" windowWidth="32664" windowHeight="19500" firstSheet="3" xr2:uid="{A813E664-7740-450B-B9AA-D361BEDD0A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Resource Digest Submission" sheetId="6" r:id="rId1"/>
@@ -35,6 +35,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="222">
   <si>
     <t>Data Catalog Submission 
 Template Version Number</t>
@@ -628,6 +630,12 @@
   </si>
   <si>
     <t>Biomedical data repositories store, organize, validate, archive, preserve, and distribute data, in compliance with the FAIR Data Principles. It is a system for storing multiple research artifacts, provided at least some of the research artifacts contain Individual Research Data. A data repository often contains artifacts from multiple studies. Some data repositories accept research datasets irrespective of the structure of those datasets; other data repositories require all research datasets to conform to a standard reference model.</t>
+  </si>
+  <si>
+    <t>Analytic Tool</t>
+  </si>
+  <si>
+    <t>Any platform, methodology, framework, or other software designed for the use of and interpretation of biomedical research data.</t>
   </si>
   <si>
     <t>One, some, every, or all without specification. This term means that the statistic value applies to the set of all values in the digest partition for the data element summarized.</t>
@@ -1011,7 +1019,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1299,7 +1307,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1310,8 +1318,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -1406,12 +1414,12 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="18.600000000000001">
+    <row r="12" spans="1:15" ht="18">
       <c r="A12" s="19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="30.95">
+    <row r="14" spans="1:15" ht="31.15">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
@@ -1509,7 +1517,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select one option. " xr:uid="{636A3986-C7F7-4241-A118-AD72E422E78F}">
           <x14:formula1>
-            <xm:f>Sheet1!$A$2:$A$6</xm:f>
+            <xm:f>Sheet1!$A$2:$A$7</xm:f>
           </x14:formula1>
           <xm:sqref>B15</xm:sqref>
         </x14:dataValidation>
@@ -1551,7 +1559,7 @@
     <col min="9" max="9" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="46.5">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="46.9">
       <c r="A1" s="15" t="s">
         <v>6</v>
       </c>
@@ -4530,10 +4538,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD15778E-9931-4B41-A419-E999FE527953}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:Y45"/>
+  <dimension ref="A1:Y46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -4597,7 +4605,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="31" customFormat="1" ht="29.1">
+    <row r="4" spans="1:5" s="31" customFormat="1" ht="28.9">
       <c r="A4" s="31" t="s">
         <v>13</v>
       </c>
@@ -4697,7 +4705,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="31" customFormat="1" ht="43.5">
+    <row r="12" spans="1:5" s="31" customFormat="1" ht="43.15">
       <c r="A12" s="31" t="s">
         <v>140</v>
       </c>
@@ -4708,7 +4716,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="31" customFormat="1" ht="29.1">
+    <row r="13" spans="1:5" s="31" customFormat="1" ht="28.9">
       <c r="A13" s="31" t="s">
         <v>140</v>
       </c>
@@ -4820,7 +4828,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="31" customFormat="1" ht="43.5">
+    <row r="21" spans="1:5" s="31" customFormat="1" ht="43.15">
       <c r="A21" s="31" t="s">
         <v>27</v>
       </c>
@@ -4831,7 +4839,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="31" customFormat="1" ht="29.1">
+    <row r="22" spans="1:5" s="31" customFormat="1" ht="28.9">
       <c r="A22" s="31" t="s">
         <v>27</v>
       </c>
@@ -4848,7 +4856,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="23" spans="1:5" s="31" customFormat="1" ht="29.1">
+    <row r="23" spans="1:5" s="31" customFormat="1" ht="28.9">
       <c r="A23" s="31" t="s">
         <v>27</v>
       </c>
@@ -4859,7 +4867,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="31" customFormat="1" ht="29.1">
+    <row r="24" spans="1:5" s="31" customFormat="1" ht="28.9">
       <c r="A24" s="31" t="s">
         <v>27</v>
       </c>
@@ -4871,7 +4879,7 @@
       </c>
       <c r="D24" s="41"/>
     </row>
-    <row r="25" spans="1:5" s="31" customFormat="1" ht="57.95">
+    <row r="25" spans="1:5" s="31" customFormat="1" ht="57.6">
       <c r="A25" s="31" t="s">
         <v>27</v>
       </c>
@@ -4905,7 +4913,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:5" s="31" customFormat="1" ht="29.1">
+    <row r="27" spans="1:5" s="31" customFormat="1" ht="28.9">
       <c r="A27" s="31" t="s">
         <v>176</v>
       </c>
@@ -4949,7 +4957,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="31" customFormat="1" ht="29.1">
+    <row r="31" spans="1:5" s="31" customFormat="1" ht="28.9">
       <c r="A31" s="31" t="s">
         <v>176</v>
       </c>
@@ -4960,7 +4968,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="31" customFormat="1" ht="29.1">
+    <row r="32" spans="1:5" s="31" customFormat="1" ht="28.9">
       <c r="A32" s="31" t="s">
         <v>176</v>
       </c>
@@ -4982,7 +4990,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="34" spans="1:5" s="31" customFormat="1" ht="57.95">
+    <row r="34" spans="1:5" s="31" customFormat="1" ht="57.6">
       <c r="A34" s="31" t="s">
         <v>12</v>
       </c>
@@ -4999,7 +5007,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="31" customFormat="1" ht="29.1">
+    <row r="35" spans="1:5" s="31" customFormat="1" ht="28.9">
       <c r="A35" s="31" t="s">
         <v>12</v>
       </c>
@@ -5016,7 +5024,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="31" customFormat="1" ht="29.1">
+    <row r="36" spans="1:5" s="31" customFormat="1" ht="28.9">
       <c r="A36" s="31" t="s">
         <v>12</v>
       </c>
@@ -5027,7 +5035,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="29.1">
+    <row r="37" spans="1:5" ht="28.9">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -5039,7 +5047,7 @@
       </c>
       <c r="E37"/>
     </row>
-    <row r="38" spans="1:5" ht="72.599999999999994">
+    <row r="38" spans="1:5" ht="72">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -5051,7 +5059,7 @@
       </c>
       <c r="E38"/>
     </row>
-    <row r="39" spans="1:5" ht="72.599999999999994">
+    <row r="39" spans="1:5" ht="72">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -5063,41 +5071,36 @@
       </c>
       <c r="E39"/>
     </row>
-    <row r="40" spans="1:5" ht="29.1">
+    <row r="40" spans="1:5" ht="30.75">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>195</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E40"/>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" ht="28.9">
       <c r="A41" t="s">
         <v>36</v>
       </c>
       <c r="B41" t="s">
-        <v>196</v>
+        <v>61</v>
       </c>
       <c r="C41" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="D41" t="s">
-        <v>126</v>
-      </c>
-      <c r="E41" t="s">
-        <v>198</v>
-      </c>
+      <c r="E41"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>40</v>
+        <v>198</v>
       </c>
       <c r="C42" s="37" t="s">
         <v>199</v>
@@ -5109,19 +5112,24 @@
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="29.1">
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>36</v>
       </c>
       <c r="B43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="C43" s="37" t="s">
+      <c r="D43" t="s">
+        <v>126</v>
+      </c>
+      <c r="E43" t="s">
         <v>202</v>
       </c>
-      <c r="E43"/>
-    </row>
-    <row r="44" spans="1:5">
+    </row>
+    <row r="44" spans="1:5" ht="28.9">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -5131,28 +5139,40 @@
       <c r="C44" s="37" t="s">
         <v>204</v>
       </c>
-      <c r="D44" t="s">
-        <v>126</v>
-      </c>
-      <c r="E44" t="s">
-        <v>205</v>
-      </c>
+      <c r="E44"/>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>36</v>
       </c>
       <c r="B45" t="s">
+        <v>205</v>
+      </c>
+      <c r="C45" s="37" t="s">
         <v>206</v>
-      </c>
-      <c r="C45" s="37" t="s">
-        <v>207</v>
       </c>
       <c r="D45" t="s">
         <v>126</v>
       </c>
       <c r="E45" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>36</v>
+      </c>
+      <c r="B46" t="s">
         <v>208</v>
+      </c>
+      <c r="C46" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="D46" t="s">
+        <v>126</v>
+      </c>
+      <c r="E46" t="s">
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -5168,7 +5188,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -5188,7 +5208,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E1" s="25" t="s">
         <v>18</v>
@@ -5213,21 +5233,21 @@
 </v>
       </c>
       <c r="D2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B3" t="s">
         <v>131</v>
@@ -5238,16 +5258,16 @@
 </v>
       </c>
       <c r="D3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="G3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -5281,7 +5301,7 @@
         <v>169</v>
       </c>
       <c r="B6" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C6" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B6&amp;" "&amp;CHAR(10)</f>
@@ -5290,7 +5310,9 @@
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="6"/>
+      <c r="A7" s="6" t="s">
+        <v>195</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5299,12 +5321,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5531,18 +5555,16 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{722799C8-19D7-48DA-861A-B77FE73B4586}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAC26B0D-F1C9-4B83-9743-12952380C0A1}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5550,5 +5572,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAC26B0D-F1C9-4B83-9743-12952380C0A1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{722799C8-19D7-48DA-861A-B77FE73B4586}"/>
 </file>
</xml_diff>

<commit_message>
Update About Page download file (Feb, 2023)
Update About Page download file (Feb, 2023)
</commit_message>
<xml_diff>
--- a/Public/Childhood_Cancer_Data_Catalog_Submission_Template.xlsx
+++ b/Public/Childhood_Cancer_Data_Catalog_Submission_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{1DBD8EDA-8D16-48B6-ABF1-40CB9C71B357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7A6E1AF-0EC4-4C7D-87EE-5B3B82C44EC2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F34F5CF1-09EF-4497-8964-B836931ECF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32892" yWindow="792" windowWidth="32664" windowHeight="19500" firstSheet="3" xr2:uid="{A813E664-7740-450B-B9AA-D361BEDD0A87}"/>
+    <workbookView xWindow="32892" yWindow="792" windowWidth="32664" windowHeight="19500" xr2:uid="{A813E664-7740-450B-B9AA-D361BEDD0A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Resource Digest Submission" sheetId="6" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="224">
   <si>
     <t>Data Catalog Submission 
 Template Version Number</t>
@@ -680,9 +680,18 @@
     <t>https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C25570</t>
   </si>
   <si>
+    <t>Epidemiologic</t>
+  </si>
+  <si>
+    <t>Relating to the study of the distribution and determinants of health-related states or events (including disease) in populations, and the application of this study to the control of diseases and other health problems</t>
+  </si>
+  <si>
     <t>Yes/No</t>
   </si>
   <si>
+    <t>Cell Lines</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -695,22 +704,19 @@
     <t>Update detected at resource site</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Mix</t>
+  </si>
+  <si>
+    <t>Data provided by resource owner</t>
+  </si>
+  <si>
+    <t>Updated provided by resource owner</t>
+  </si>
+  <si>
     <t>Knowledgebase</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Mix</t>
-  </si>
-  <si>
-    <t>Data provided by resource owner</t>
-  </si>
-  <si>
-    <t>Updated provided by resource owner</t>
-  </si>
-  <si>
-    <t>Cell Lines</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1025,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1307,7 +1313,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1318,8 +1324,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -1499,7 +1505,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="711" yWindow="709" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select all applicable options." xr:uid="{24609F91-DD67-4A61-931E-EC1E776B8001}">
           <x14:formula1>
-            <xm:f>Sheet1!$C$2:$C$6</xm:f>
+            <xm:f>Sheet1!$C$2:$C$7</xm:f>
           </x14:formula1>
           <xm:sqref>C15</xm:sqref>
         </x14:dataValidation>
@@ -4538,10 +4544,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD15778E-9931-4B41-A419-E999FE527953}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:Y46"/>
+  <dimension ref="A1:Y47"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -4554,7 +4560,7 @@
     <col min="6" max="25" width="8.85546875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="33" customFormat="1">
+    <row r="1" spans="1:5" s="33" customFormat="1" ht="15">
       <c r="A1" s="14" t="s">
         <v>120</v>
       </c>
@@ -5175,8 +5181,19 @@
         <v>210</v>
       </c>
     </row>
+    <row r="47" spans="1:5" ht="30.75">
+      <c r="A47" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" t="s">
+        <v>211</v>
+      </c>
+      <c r="C47" s="37" t="s">
+        <v>212</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{CD15778E-9931-4B41-A419-E999FE527953}"/>
+  <autoFilter ref="A1:E47" xr:uid="{CD15778E-9931-4B41-A419-E999FE527953}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
@@ -5188,7 +5205,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -5208,7 +5225,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E1" s="25" t="s">
         <v>18</v>
@@ -5222,116 +5239,116 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>214</v>
       </c>
       <c r="C2" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B2&amp;" "&amp;CHAR(10)</f>
+        <v xml:space="preserve">Cell Lines 
+</v>
+      </c>
+      <c r="D2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B3&amp;" "&amp;CHAR(10)</f>
+        <v xml:space="preserve">Clinical 
+</v>
+      </c>
+      <c r="D3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C4" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B4&amp;" "&amp;CHAR(10)</f>
+        <v xml:space="preserve">Epidemiologic 
+</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B5&amp;" "&amp;CHAR(10)</f>
         <v xml:space="preserve">Genomics/Omics 
 </v>
       </c>
-      <c r="D2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E2" t="s">
-        <v>213</v>
-      </c>
-      <c r="F2" t="s">
-        <v>214</v>
-      </c>
-      <c r="G2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" t="s">
         <v>131</v>
       </c>
-      <c r="C3" t="str">
-        <f>'Data Resource Digest Submission'!$C$15&amp;B3&amp;" "&amp;CHAR(10)</f>
+      <c r="C6" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B6&amp;" "&amp;CHAR(10)</f>
         <v xml:space="preserve">Imaging 
 </v>
       </c>
-      <c r="D3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E3" t="s">
-        <v>218</v>
-      </c>
-      <c r="F3" t="s">
-        <v>219</v>
-      </c>
-      <c r="G3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="B4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" t="str">
-        <f>'Data Resource Digest Submission'!$C$15&amp;B4&amp;" "&amp;CHAR(10)</f>
-        <v xml:space="preserve">Clinical 
-</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="6" t="s">
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>137</v>
       </c>
-      <c r="C5" t="str">
-        <f>'Data Resource Digest Submission'!$C$15&amp;B5&amp;" "&amp;CHAR(10)</f>
+      <c r="C7" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B7&amp;" "&amp;CHAR(10)</f>
         <v xml:space="preserve">Xenograft 
 </v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C6" t="str">
-        <f>'Data Resource Digest Submission'!$C$15&amp;B6&amp;" "&amp;CHAR(10)</f>
-        <v xml:space="preserve">Cell Lines 
-</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A7">
+    <sortCondition ref="A2:A7"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d54ef3ca738e332da14dc10991e335">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2789f7211f2f0296d09b7bbdbdf6676" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -5554,6 +5571,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5564,11 +5592,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAC26B0D-F1C9-4B83-9743-12952380C0A1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8CA60CD-2286-4C35-8489-90021763D1F5}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8CA60CD-2286-4C35-8489-90021763D1F5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAC26B0D-F1C9-4B83-9743-12952380C0A1}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Update About Page download file (Feb, 2023) (#77)
Update About Page download file (Feb, 2023)
</commit_message>
<xml_diff>
--- a/Public/Childhood_Cancer_Data_Catalog_Submission_Template.xlsx
+++ b/Public/Childhood_Cancer_Data_Catalog_Submission_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{1DBD8EDA-8D16-48B6-ABF1-40CB9C71B357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7A6E1AF-0EC4-4C7D-87EE-5B3B82C44EC2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F34F5CF1-09EF-4497-8964-B836931ECF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32892" yWindow="792" windowWidth="32664" windowHeight="19500" firstSheet="3" xr2:uid="{A813E664-7740-450B-B9AA-D361BEDD0A87}"/>
+    <workbookView xWindow="32892" yWindow="792" windowWidth="32664" windowHeight="19500" xr2:uid="{A813E664-7740-450B-B9AA-D361BEDD0A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Resource Digest Submission" sheetId="6" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="224">
   <si>
     <t>Data Catalog Submission 
 Template Version Number</t>
@@ -680,9 +680,18 @@
     <t>https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C25570</t>
   </si>
   <si>
+    <t>Epidemiologic</t>
+  </si>
+  <si>
+    <t>Relating to the study of the distribution and determinants of health-related states or events (including disease) in populations, and the application of this study to the control of diseases and other health problems</t>
+  </si>
+  <si>
     <t>Yes/No</t>
   </si>
   <si>
+    <t>Cell Lines</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -695,22 +704,19 @@
     <t>Update detected at resource site</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Mix</t>
+  </si>
+  <si>
+    <t>Data provided by resource owner</t>
+  </si>
+  <si>
+    <t>Updated provided by resource owner</t>
+  </si>
+  <si>
     <t>Knowledgebase</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Mix</t>
-  </si>
-  <si>
-    <t>Data provided by resource owner</t>
-  </si>
-  <si>
-    <t>Updated provided by resource owner</t>
-  </si>
-  <si>
-    <t>Cell Lines</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1025,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1307,7 +1313,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1318,8 +1324,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -1499,7 +1505,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="711" yWindow="709" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select all applicable options." xr:uid="{24609F91-DD67-4A61-931E-EC1E776B8001}">
           <x14:formula1>
-            <xm:f>Sheet1!$C$2:$C$6</xm:f>
+            <xm:f>Sheet1!$C$2:$C$7</xm:f>
           </x14:formula1>
           <xm:sqref>C15</xm:sqref>
         </x14:dataValidation>
@@ -4538,10 +4544,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD15778E-9931-4B41-A419-E999FE527953}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:Y46"/>
+  <dimension ref="A1:Y47"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -4554,7 +4560,7 @@
     <col min="6" max="25" width="8.85546875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="33" customFormat="1">
+    <row r="1" spans="1:5" s="33" customFormat="1" ht="15">
       <c r="A1" s="14" t="s">
         <v>120</v>
       </c>
@@ -5175,8 +5181,19 @@
         <v>210</v>
       </c>
     </row>
+    <row r="47" spans="1:5" ht="30.75">
+      <c r="A47" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" t="s">
+        <v>211</v>
+      </c>
+      <c r="C47" s="37" t="s">
+        <v>212</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{CD15778E-9931-4B41-A419-E999FE527953}"/>
+  <autoFilter ref="A1:E47" xr:uid="{CD15778E-9931-4B41-A419-E999FE527953}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
@@ -5188,7 +5205,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -5208,7 +5225,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E1" s="25" t="s">
         <v>18</v>
@@ -5222,116 +5239,116 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>214</v>
       </c>
       <c r="C2" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B2&amp;" "&amp;CHAR(10)</f>
+        <v xml:space="preserve">Cell Lines 
+</v>
+      </c>
+      <c r="D2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B3&amp;" "&amp;CHAR(10)</f>
+        <v xml:space="preserve">Clinical 
+</v>
+      </c>
+      <c r="D3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C4" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B4&amp;" "&amp;CHAR(10)</f>
+        <v xml:space="preserve">Epidemiologic 
+</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B5&amp;" "&amp;CHAR(10)</f>
         <v xml:space="preserve">Genomics/Omics 
 </v>
       </c>
-      <c r="D2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E2" t="s">
-        <v>213</v>
-      </c>
-      <c r="F2" t="s">
-        <v>214</v>
-      </c>
-      <c r="G2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" t="s">
         <v>131</v>
       </c>
-      <c r="C3" t="str">
-        <f>'Data Resource Digest Submission'!$C$15&amp;B3&amp;" "&amp;CHAR(10)</f>
+      <c r="C6" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B6&amp;" "&amp;CHAR(10)</f>
         <v xml:space="preserve">Imaging 
 </v>
       </c>
-      <c r="D3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E3" t="s">
-        <v>218</v>
-      </c>
-      <c r="F3" t="s">
-        <v>219</v>
-      </c>
-      <c r="G3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="B4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" t="str">
-        <f>'Data Resource Digest Submission'!$C$15&amp;B4&amp;" "&amp;CHAR(10)</f>
-        <v xml:space="preserve">Clinical 
-</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="6" t="s">
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>137</v>
       </c>
-      <c r="C5" t="str">
-        <f>'Data Resource Digest Submission'!$C$15&amp;B5&amp;" "&amp;CHAR(10)</f>
+      <c r="C7" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B7&amp;" "&amp;CHAR(10)</f>
         <v xml:space="preserve">Xenograft 
 </v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C6" t="str">
-        <f>'Data Resource Digest Submission'!$C$15&amp;B6&amp;" "&amp;CHAR(10)</f>
-        <v xml:space="preserve">Cell Lines 
-</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A7">
+    <sortCondition ref="A2:A7"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d54ef3ca738e332da14dc10991e335">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2789f7211f2f0296d09b7bbdbdf6676" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -5554,6 +5571,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5564,11 +5592,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAC26B0D-F1C9-4B83-9743-12952380C0A1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8CA60CD-2286-4C35-8489-90021763D1F5}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8CA60CD-2286-4C35-8489-90021763D1F5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAC26B0D-F1C9-4B83-9743-12952380C0A1}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Update About Page download file (Feb, 2023) (#77) (#78)
Update About Page download file (Feb, 2023)

Co-authored-by: Ruoxi Zhang <116577061+RuoxiZhang08@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Public/Childhood_Cancer_Data_Catalog_Submission_Template.xlsx
+++ b/Public/Childhood_Cancer_Data_Catalog_Submission_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{1DBD8EDA-8D16-48B6-ABF1-40CB9C71B357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7A6E1AF-0EC4-4C7D-87EE-5B3B82C44EC2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F34F5CF1-09EF-4497-8964-B836931ECF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32892" yWindow="792" windowWidth="32664" windowHeight="19500" firstSheet="3" xr2:uid="{A813E664-7740-450B-B9AA-D361BEDD0A87}"/>
+    <workbookView xWindow="32892" yWindow="792" windowWidth="32664" windowHeight="19500" xr2:uid="{A813E664-7740-450B-B9AA-D361BEDD0A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Resource Digest Submission" sheetId="6" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="224">
   <si>
     <t>Data Catalog Submission 
 Template Version Number</t>
@@ -680,9 +680,18 @@
     <t>https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C25570</t>
   </si>
   <si>
+    <t>Epidemiologic</t>
+  </si>
+  <si>
+    <t>Relating to the study of the distribution and determinants of health-related states or events (including disease) in populations, and the application of this study to the control of diseases and other health problems</t>
+  </si>
+  <si>
     <t>Yes/No</t>
   </si>
   <si>
+    <t>Cell Lines</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -695,22 +704,19 @@
     <t>Update detected at resource site</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Mix</t>
+  </si>
+  <si>
+    <t>Data provided by resource owner</t>
+  </si>
+  <si>
+    <t>Updated provided by resource owner</t>
+  </si>
+  <si>
     <t>Knowledgebase</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Mix</t>
-  </si>
-  <si>
-    <t>Data provided by resource owner</t>
-  </si>
-  <si>
-    <t>Updated provided by resource owner</t>
-  </si>
-  <si>
-    <t>Cell Lines</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1025,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1307,7 +1313,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1318,8 +1324,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -1499,7 +1505,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="711" yWindow="709" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select all applicable options." xr:uid="{24609F91-DD67-4A61-931E-EC1E776B8001}">
           <x14:formula1>
-            <xm:f>Sheet1!$C$2:$C$6</xm:f>
+            <xm:f>Sheet1!$C$2:$C$7</xm:f>
           </x14:formula1>
           <xm:sqref>C15</xm:sqref>
         </x14:dataValidation>
@@ -4538,10 +4544,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD15778E-9931-4B41-A419-E999FE527953}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:Y46"/>
+  <dimension ref="A1:Y47"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -4554,7 +4560,7 @@
     <col min="6" max="25" width="8.85546875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="33" customFormat="1">
+    <row r="1" spans="1:5" s="33" customFormat="1" ht="15">
       <c r="A1" s="14" t="s">
         <v>120</v>
       </c>
@@ -5175,8 +5181,19 @@
         <v>210</v>
       </c>
     </row>
+    <row r="47" spans="1:5" ht="30.75">
+      <c r="A47" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" t="s">
+        <v>211</v>
+      </c>
+      <c r="C47" s="37" t="s">
+        <v>212</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{CD15778E-9931-4B41-A419-E999FE527953}"/>
+  <autoFilter ref="A1:E47" xr:uid="{CD15778E-9931-4B41-A419-E999FE527953}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
@@ -5188,7 +5205,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -5208,7 +5225,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E1" s="25" t="s">
         <v>18</v>
@@ -5222,116 +5239,116 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>214</v>
       </c>
       <c r="C2" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B2&amp;" "&amp;CHAR(10)</f>
+        <v xml:space="preserve">Cell Lines 
+</v>
+      </c>
+      <c r="D2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B3&amp;" "&amp;CHAR(10)</f>
+        <v xml:space="preserve">Clinical 
+</v>
+      </c>
+      <c r="D3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C4" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B4&amp;" "&amp;CHAR(10)</f>
+        <v xml:space="preserve">Epidemiologic 
+</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B5&amp;" "&amp;CHAR(10)</f>
         <v xml:space="preserve">Genomics/Omics 
 </v>
       </c>
-      <c r="D2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E2" t="s">
-        <v>213</v>
-      </c>
-      <c r="F2" t="s">
-        <v>214</v>
-      </c>
-      <c r="G2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" t="s">
         <v>131</v>
       </c>
-      <c r="C3" t="str">
-        <f>'Data Resource Digest Submission'!$C$15&amp;B3&amp;" "&amp;CHAR(10)</f>
+      <c r="C6" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B6&amp;" "&amp;CHAR(10)</f>
         <v xml:space="preserve">Imaging 
 </v>
       </c>
-      <c r="D3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E3" t="s">
-        <v>218</v>
-      </c>
-      <c r="F3" t="s">
-        <v>219</v>
-      </c>
-      <c r="G3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="B4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" t="str">
-        <f>'Data Resource Digest Submission'!$C$15&amp;B4&amp;" "&amp;CHAR(10)</f>
-        <v xml:space="preserve">Clinical 
-</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="6" t="s">
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>137</v>
       </c>
-      <c r="C5" t="str">
-        <f>'Data Resource Digest Submission'!$C$15&amp;B5&amp;" "&amp;CHAR(10)</f>
+      <c r="C7" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B7&amp;" "&amp;CHAR(10)</f>
         <v xml:space="preserve">Xenograft 
 </v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C6" t="str">
-        <f>'Data Resource Digest Submission'!$C$15&amp;B6&amp;" "&amp;CHAR(10)</f>
-        <v xml:space="preserve">Cell Lines 
-</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A7">
+    <sortCondition ref="A2:A7"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d54ef3ca738e332da14dc10991e335">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2789f7211f2f0296d09b7bbdbdf6676" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -5554,6 +5571,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5564,11 +5592,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAC26B0D-F1C9-4B83-9743-12952380C0A1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8CA60CD-2286-4C35-8489-90021763D1F5}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8CA60CD-2286-4C35-8489-90021763D1F5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAC26B0D-F1C9-4B83-9743-12952380C0A1}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Update About Page download file (Feb, 2023) (#77) (#78) (#79)
Update About Page download file (Feb, 2023)

Co-authored-by: Ruoxi Zhang <116577061+RuoxiZhang08@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Public/Childhood_Cancer_Data_Catalog_Submission_Template.xlsx
+++ b/Public/Childhood_Cancer_Data_Catalog_Submission_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{1DBD8EDA-8D16-48B6-ABF1-40CB9C71B357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7A6E1AF-0EC4-4C7D-87EE-5B3B82C44EC2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F34F5CF1-09EF-4497-8964-B836931ECF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32892" yWindow="792" windowWidth="32664" windowHeight="19500" firstSheet="3" xr2:uid="{A813E664-7740-450B-B9AA-D361BEDD0A87}"/>
+    <workbookView xWindow="32892" yWindow="792" windowWidth="32664" windowHeight="19500" xr2:uid="{A813E664-7740-450B-B9AA-D361BEDD0A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Resource Digest Submission" sheetId="6" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="224">
   <si>
     <t>Data Catalog Submission 
 Template Version Number</t>
@@ -680,9 +680,18 @@
     <t>https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C25570</t>
   </si>
   <si>
+    <t>Epidemiologic</t>
+  </si>
+  <si>
+    <t>Relating to the study of the distribution and determinants of health-related states or events (including disease) in populations, and the application of this study to the control of diseases and other health problems</t>
+  </si>
+  <si>
     <t>Yes/No</t>
   </si>
   <si>
+    <t>Cell Lines</t>
+  </si>
+  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -695,22 +704,19 @@
     <t>Update detected at resource site</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Mix</t>
+  </si>
+  <si>
+    <t>Data provided by resource owner</t>
+  </si>
+  <si>
+    <t>Updated provided by resource owner</t>
+  </si>
+  <si>
     <t>Knowledgebase</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Mix</t>
-  </si>
-  <si>
-    <t>Data provided by resource owner</t>
-  </si>
-  <si>
-    <t>Updated provided by resource owner</t>
-  </si>
-  <si>
-    <t>Cell Lines</t>
   </si>
 </sst>
 </file>
@@ -1019,7 +1025,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1307,7 +1313,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1318,8 +1324,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -1499,7 +1505,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="711" yWindow="709" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select all applicable options." xr:uid="{24609F91-DD67-4A61-931E-EC1E776B8001}">
           <x14:formula1>
-            <xm:f>Sheet1!$C$2:$C$6</xm:f>
+            <xm:f>Sheet1!$C$2:$C$7</xm:f>
           </x14:formula1>
           <xm:sqref>C15</xm:sqref>
         </x14:dataValidation>
@@ -4538,10 +4544,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD15778E-9931-4B41-A419-E999FE527953}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:Y46"/>
+  <dimension ref="A1:Y47"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -4554,7 +4560,7 @@
     <col min="6" max="25" width="8.85546875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="33" customFormat="1">
+    <row r="1" spans="1:5" s="33" customFormat="1" ht="15">
       <c r="A1" s="14" t="s">
         <v>120</v>
       </c>
@@ -5175,8 +5181,19 @@
         <v>210</v>
       </c>
     </row>
+    <row r="47" spans="1:5" ht="30.75">
+      <c r="A47" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" t="s">
+        <v>211</v>
+      </c>
+      <c r="C47" s="37" t="s">
+        <v>212</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{CD15778E-9931-4B41-A419-E999FE527953}"/>
+  <autoFilter ref="A1:E47" xr:uid="{CD15778E-9931-4B41-A419-E999FE527953}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
@@ -5188,7 +5205,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -5208,7 +5225,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E1" s="25" t="s">
         <v>18</v>
@@ -5222,116 +5239,116 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>214</v>
       </c>
       <c r="C2" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B2&amp;" "&amp;CHAR(10)</f>
+        <v xml:space="preserve">Cell Lines 
+</v>
+      </c>
+      <c r="D2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B3&amp;" "&amp;CHAR(10)</f>
+        <v xml:space="preserve">Clinical 
+</v>
+      </c>
+      <c r="D3" t="s">
+        <v>219</v>
+      </c>
+      <c r="E3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="B4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C4" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B4&amp;" "&amp;CHAR(10)</f>
+        <v xml:space="preserve">Epidemiologic 
+</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B5&amp;" "&amp;CHAR(10)</f>
         <v xml:space="preserve">Genomics/Omics 
 </v>
       </c>
-      <c r="D2" t="s">
-        <v>212</v>
-      </c>
-      <c r="E2" t="s">
-        <v>213</v>
-      </c>
-      <c r="F2" t="s">
-        <v>214</v>
-      </c>
-      <c r="G2" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" t="s">
         <v>131</v>
       </c>
-      <c r="C3" t="str">
-        <f>'Data Resource Digest Submission'!$C$15&amp;B3&amp;" "&amp;CHAR(10)</f>
+      <c r="C6" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B6&amp;" "&amp;CHAR(10)</f>
         <v xml:space="preserve">Imaging 
 </v>
       </c>
-      <c r="D3" t="s">
-        <v>217</v>
-      </c>
-      <c r="E3" t="s">
-        <v>218</v>
-      </c>
-      <c r="F3" t="s">
-        <v>219</v>
-      </c>
-      <c r="G3" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="B4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" t="str">
-        <f>'Data Resource Digest Submission'!$C$15&amp;B4&amp;" "&amp;CHAR(10)</f>
-        <v xml:space="preserve">Clinical 
-</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="6" t="s">
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>137</v>
       </c>
-      <c r="C5" t="str">
-        <f>'Data Resource Digest Submission'!$C$15&amp;B5&amp;" "&amp;CHAR(10)</f>
+      <c r="C7" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B7&amp;" "&amp;CHAR(10)</f>
         <v xml:space="preserve">Xenograft 
 </v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B6" t="s">
-        <v>221</v>
-      </c>
-      <c r="C6" t="str">
-        <f>'Data Resource Digest Submission'!$C$15&amp;B6&amp;" "&amp;CHAR(10)</f>
-        <v xml:space="preserve">Cell Lines 
-</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="6" t="s">
-        <v>195</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A7">
+    <sortCondition ref="A2:A7"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d54ef3ca738e332da14dc10991e335">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2789f7211f2f0296d09b7bbdbdf6676" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
@@ -5554,6 +5571,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="33e70369-3675-4c3b-99e1-030eb9633bdf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5564,11 +5592,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAC26B0D-F1C9-4B83-9743-12952380C0A1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8CA60CD-2286-4C35-8489-90021763D1F5}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8CA60CD-2286-4C35-8489-90021763D1F5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAC26B0D-F1C9-4B83-9743-12952380C0A1}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
PODCAT-1178: update submission template
</commit_message>
<xml_diff>
--- a/Public/Childhood_Cancer_Data_Catalog_Submission_Template.xlsx
+++ b/Public/Childhood_Cancer_Data_Catalog_Submission_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26727"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nih.sharepoint.com/sites/NCI-CBIIT-FNLCCDI/Shared Documents/CCDC (Data Catalog nee PODCat)/2-Executing/System Document/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F34F5CF1-09EF-4497-8964-B836931ECF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE9A20E7-BF8D-4864-A084-1730E6915D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32892" yWindow="792" windowWidth="32664" windowHeight="19500" xr2:uid="{A813E664-7740-450B-B9AA-D361BEDD0A87}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A813E664-7740-450B-B9AA-D361BEDD0A87}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Resource Digest Submission" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Digest 1'!$A$1:$H$98</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Glossary!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Glossary!$A$1:$E$49</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -44,13 +44,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="230">
   <si>
     <t>Data Catalog Submission 
 Template Version Number</t>
   </si>
   <si>
-    <t>Version 3.6</t>
+    <t>Version 3.7</t>
   </si>
   <si>
     <t xml:space="preserve">This is a submission template for use in submitting Childhood Cancer Data Digests for the Childhood Cancer Data Catalog.  For instructions on filling out this workbooks and information on submitting dataset digests to the Childhood Cancer Data Catalog, contact Subhashini Jagu (subhashini.jagu@nih.gov) from NCI's Office of Data Sharing (ODS). </t>
@@ -467,6 +467,21 @@
     <t>https://www.cancer.gov/publications/dictionaries/cancer-terms/def/xenograft</t>
   </si>
   <si>
+    <t>Epidemiologic</t>
+  </si>
+  <si>
+    <t>Relating to the study of the distribution and determinants of health-related states or events (including disease) in populations, and the application of this study to the control of diseases and other health problems</t>
+  </si>
+  <si>
+    <t>Biospecimen</t>
+  </si>
+  <si>
+    <t>A sample of material, such as urine, blood, tissue, cells, DNA, RNA, or protein, from humans, animals, or plants. Biospecimens may be used for a laboratory test or stored in a biorepository to be used for research.</t>
+  </si>
+  <si>
+    <t>https://www.cancer.gov/publications/dictionaries/cancer-terms/def/biospecimen</t>
+  </si>
+  <si>
     <t>Dataset Structure</t>
   </si>
   <si>
@@ -626,7 +641,7 @@
     <t>A cancer registry is an information system designed for the collection, storage, and management of data on persons with cancer. An inventory of individuals or samples, usually focused on a specific diagnosis or condition. In some cases, public health laws require collecting information in registries about individuals who have a specific disease or condition. In other cases, individuals provide information about themselves to these registries voluntarily. Thus, a registry contains Individual Clinical Data, but not Individual Research Data.</t>
   </si>
   <si>
-    <t>Repository</t>
+    <t>Data Repository</t>
   </si>
   <si>
     <t>Biomedical data repositories store, organize, validate, archive, preserve, and distribute data, in compliance with the FAIR Data Principles. It is a system for storing multiple research artifacts, provided at least some of the research artifacts contain Individual Research Data. A data repository often contains artifacts from multiple studies. Some data repositories accept research datasets irrespective of the structure of those datasets; other data repositories require all research datasets to conform to a standard reference model.</t>
@@ -638,6 +653,15 @@
     <t>Any platform, methodology, framework, or other software designed for the use of and interpretation of biomedical research data.</t>
   </si>
   <si>
+    <t>Biorepository</t>
+  </si>
+  <si>
+    <t>A biorepository is a facility that acts as a library for biospecimens, allowing the biospecimens to be available for use in future research. A biospecimen may be from people, animals, or other living organisms. A biorepository will be involved in collecting, cataloguing, and storing biospecimens. The biorepository will also be involved in managing access to and distributing biospecimens to researchers. Some biorepositories store medical information associated with biospecimens.</t>
+  </si>
+  <si>
+    <t>https://toolkit.ncats.nih.gov/glossary/biorepository/</t>
+  </si>
+  <si>
     <t>One, some, every, or all without specification. This term means that the statistic value applies to the set of all values in the digest partition for the data element summarized.</t>
   </si>
   <si>
@@ -678,12 +702,6 @@
   </si>
   <si>
     <t>https://ncithesaurus.nci.nih.gov/ncitbrowser/ConceptReport.jsp?dictionary=NCI_Thesaurus&amp;ns=ncit&amp;code=C25570</t>
-  </si>
-  <si>
-    <t>Epidemiologic</t>
-  </si>
-  <si>
-    <t>Relating to the study of the distribution and determinants of health-related states or events (including disease) in populations, and the application of this study to the control of diseases and other health problems</t>
   </si>
   <si>
     <t>Yes/No</t>
@@ -1324,8 +1342,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -1420,12 +1438,12 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="18">
+    <row r="12" spans="1:15" ht="18.600000000000001">
       <c r="A12" s="19" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="31.15">
+    <row r="14" spans="1:15" ht="30.95">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
@@ -1505,7 +1523,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="711" yWindow="709" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select all applicable options." xr:uid="{24609F91-DD67-4A61-931E-EC1E776B8001}">
           <x14:formula1>
-            <xm:f>Sheet1!$C$2:$C$7</xm:f>
+            <xm:f>Sheet1!$C$2:$C$8</xm:f>
           </x14:formula1>
           <xm:sqref>C15</xm:sqref>
         </x14:dataValidation>
@@ -1523,7 +1541,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select one option. " xr:uid="{636A3986-C7F7-4241-A118-AD72E422E78F}">
           <x14:formula1>
-            <xm:f>Sheet1!$A$2:$A$7</xm:f>
+            <xm:f>Sheet1!$A$2:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>B15</xm:sqref>
         </x14:dataValidation>
@@ -1565,7 +1583,7 @@
     <col min="9" max="9" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="46.9">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="46.5">
       <c r="A1" s="15" t="s">
         <v>6</v>
       </c>
@@ -4544,10 +4562,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD15778E-9931-4B41-A419-E999FE527953}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:Y47"/>
+  <dimension ref="A1:Y49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -4560,7 +4578,7 @@
     <col min="6" max="25" width="8.85546875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="33" customFormat="1" ht="15">
+    <row r="1" spans="1:5" s="33" customFormat="1">
       <c r="A1" s="14" t="s">
         <v>120</v>
       </c>
@@ -4611,7 +4629,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="31" customFormat="1" ht="28.9">
+    <row r="4" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A4" s="31" t="s">
         <v>13</v>
       </c>
@@ -4656,106 +4674,107 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="31" customFormat="1">
+    <row r="7" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A7" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>140</v>
       </c>
-      <c r="B7" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="37" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" s="31" customFormat="1">
+      <c r="D7"/>
+    </row>
+    <row r="8" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A8" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
         <v>142</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="31" customFormat="1">
       <c r="A9" s="31" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="31" customFormat="1">
       <c r="A10" s="31" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>144</v>
+        <v>26</v>
       </c>
       <c r="C10" s="39" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="31" customFormat="1">
       <c r="A11" s="31" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B11" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="39" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="31" customFormat="1">
+      <c r="A12" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="31" customFormat="1">
+      <c r="A13" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="39" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="31" customFormat="1" ht="43.15">
-      <c r="A12" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="B12" s="31" t="s">
+      <c r="C13" s="39" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="31" customFormat="1" ht="43.5">
+      <c r="A14" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="39" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="31" customFormat="1" ht="28.9">
-      <c r="A13" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="B13" s="31" t="s">
+      <c r="C14" s="39" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="31" customFormat="1" ht="29.1">
+      <c r="A15" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" s="31" t="s">
         <v>30</v>
-      </c>
-      <c r="C13" s="39" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="31" customFormat="1">
-      <c r="A14" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="B14" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>150</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="E14" s="31" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="31" customFormat="1">
-      <c r="A15" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="31" t="s">
-        <v>152</v>
       </c>
       <c r="C15" s="39" t="s">
         <v>153</v>
@@ -4763,7 +4782,7 @@
     </row>
     <row r="16" spans="1:5" s="31" customFormat="1">
       <c r="A16" s="31" t="s">
-        <v>18</v>
+        <v>145</v>
       </c>
       <c r="B16" s="31" t="s">
         <v>154</v>
@@ -4771,39 +4790,33 @@
       <c r="C16" s="39" t="s">
         <v>155</v>
       </c>
+      <c r="D16" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" s="31" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="17" spans="1:5" s="31" customFormat="1">
       <c r="A17" s="31" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C17" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="E17" s="31" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="31" customFormat="1">
       <c r="A18" s="31" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B18" s="31" t="s">
         <v>159</v>
       </c>
       <c r="C18" s="39" t="s">
         <v>160</v>
-      </c>
-      <c r="D18" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="E18" s="31" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="31" customFormat="1">
@@ -4811,9 +4824,15 @@
         <v>27</v>
       </c>
       <c r="B19" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="C19" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="D19" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="E19" s="31" t="s">
         <v>163</v>
       </c>
     </row>
@@ -4822,47 +4841,47 @@
         <v>27</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>124</v>
+        <v>164</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>125</v>
+        <v>165</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="31" customFormat="1" ht="43.15">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="31" customFormat="1">
       <c r="A21" s="31" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="31" customFormat="1" ht="28.9">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="31" customFormat="1">
       <c r="A22" s="31" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>166</v>
+        <v>124</v>
       </c>
       <c r="C22" s="39" t="s">
-        <v>167</v>
+        <v>125</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="31" customFormat="1" ht="28.9">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="31" customFormat="1" ht="43.5">
       <c r="A23" s="31" t="s">
         <v>27</v>
       </c>
@@ -4873,277 +4892,277 @@
         <v>170</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="31" customFormat="1" ht="28.9">
+    <row r="24" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A24" s="31" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="C24" s="40" t="s">
+      <c r="C24" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="D24" s="41"/>
-    </row>
-    <row r="25" spans="1:5" s="31" customFormat="1" ht="57.6">
+      <c r="D24" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="E24" s="31" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A25" s="31" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C25" s="39" t="s">
-        <v>174</v>
-      </c>
-      <c r="D25" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="E25" s="31" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="31" customFormat="1">
+    <row r="26" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A26" s="31" t="s">
         <v>27</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="C26" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="D26" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="E26" s="31" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="31" customFormat="1" ht="28.9">
+        <v>176</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="D26" s="41"/>
+    </row>
+    <row r="27" spans="1:5" s="31" customFormat="1" ht="57.95">
       <c r="A27" s="31" t="s">
-        <v>176</v>
+        <v>27</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>13</v>
+        <v>178</v>
       </c>
       <c r="C27" s="39" t="s">
-        <v>177</v>
+        <v>179</v>
+      </c>
+      <c r="D27" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="E27" s="31" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:5" s="31" customFormat="1">
       <c r="A28" s="31" t="s">
-        <v>176</v>
+        <v>27</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>11</v>
+        <v>137</v>
       </c>
       <c r="C28" s="39" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="31" customFormat="1">
+        <v>138</v>
+      </c>
+      <c r="D28" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="E28" s="31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="31" customFormat="1" ht="29.1">
       <c r="A29" s="31" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="31" customFormat="1">
       <c r="A30" s="31" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B30" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="39" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="31" customFormat="1">
+      <c r="A31" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="39" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="31" customFormat="1">
+      <c r="A32" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="B32" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="39" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="31" customFormat="1" ht="28.9">
-      <c r="A31" s="31" t="s">
-        <v>176</v>
-      </c>
-      <c r="B31" s="31" t="s">
+      <c r="C32" s="39" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="31" customFormat="1" ht="29.1">
+      <c r="A33" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="39" t="s">
+      <c r="C33" s="39" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="31" customFormat="1" ht="29.1">
+      <c r="A34" s="31" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" s="31" customFormat="1" ht="28.9">
-      <c r="A32" s="31" t="s">
-        <v>176</v>
-      </c>
-      <c r="B32" s="31" t="s">
+      <c r="B34" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="39" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="31" customFormat="1">
-      <c r="A33" s="31" t="s">
-        <v>176</v>
-      </c>
-      <c r="B33" s="31" t="s">
+      <c r="C34" s="39" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="31" customFormat="1">
+      <c r="A35" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="B35" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="39" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="31" customFormat="1" ht="57.6">
-      <c r="A34" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="31" t="s">
-        <v>184</v>
-      </c>
-      <c r="C34" s="39" t="s">
-        <v>185</v>
-      </c>
-      <c r="D34" s="31" t="s">
-        <v>186</v>
-      </c>
-      <c r="E34" s="31" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="31" customFormat="1" ht="28.9">
-      <c r="A35" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="31" t="s">
+      <c r="C35" s="39" t="s">
         <v>188</v>
       </c>
-      <c r="C35" s="39" t="s">
-        <v>189</v>
-      </c>
-      <c r="D35" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="E35" s="31" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="31" customFormat="1" ht="28.9">
+    </row>
+    <row r="36" spans="1:5" s="31" customFormat="1" ht="57.95">
       <c r="A36" s="31" t="s">
         <v>12</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c r="C36" s="39" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="28.9">
-      <c r="A37" t="s">
+        <v>190</v>
+      </c>
+      <c r="D36" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="E36" s="31" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="31" customFormat="1" ht="29.1">
+      <c r="A37" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B37" t="s">
-        <v>171</v>
-      </c>
-      <c r="C37" s="37" t="s">
-        <v>172</v>
-      </c>
-      <c r="E37"/>
-    </row>
-    <row r="38" spans="1:5" ht="72">
-      <c r="A38" t="s">
+      <c r="B37" s="31" t="s">
+        <v>193</v>
+      </c>
+      <c r="C37" s="39" t="s">
+        <v>194</v>
+      </c>
+      <c r="D37" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="E37" s="31" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="29.1">
+      <c r="A38" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B38" t="s">
-        <v>191</v>
-      </c>
-      <c r="C38" s="37" t="s">
-        <v>192</v>
-      </c>
-      <c r="E38"/>
-    </row>
-    <row r="39" spans="1:5" ht="72">
+      <c r="B38" s="31" t="s">
+        <v>174</v>
+      </c>
+      <c r="C38" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="D38" s="31"/>
+    </row>
+    <row r="39" spans="1:5" ht="29.1">
       <c r="A39" t="s">
         <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="C39" s="37" t="s">
-        <v>194</v>
+        <v>177</v>
       </c>
       <c r="E39"/>
     </row>
-    <row r="40" spans="1:5" ht="30.75">
+    <row r="40" spans="1:5" ht="72.599999999999994">
       <c r="A40" t="s">
         <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C40" s="37" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E40"/>
     </row>
-    <row r="41" spans="1:5" ht="28.9">
+    <row r="41" spans="1:5" ht="72.599999999999994">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>198</v>
       </c>
       <c r="C41" s="37" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E41"/>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" ht="29.1">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B42" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C42" s="37" t="s">
-        <v>199</v>
-      </c>
-      <c r="D42" t="s">
-        <v>126</v>
-      </c>
-      <c r="E42" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>201</v>
+      </c>
+      <c r="E42"/>
+    </row>
+    <row r="43" spans="1:5" ht="57.95">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>202</v>
       </c>
       <c r="C43" s="37" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D43" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="E43" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="28.9">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="29.1">
       <c r="A44" t="s">
         <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>203</v>
+        <v>61</v>
       </c>
       <c r="C44" s="37" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E44"/>
     </row>
@@ -5152,16 +5171,16 @@
         <v>36</v>
       </c>
       <c r="B45" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C45" s="37" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D45" t="s">
         <v>126</v>
       </c>
       <c r="E45" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -5169,7 +5188,7 @@
         <v>36</v>
       </c>
       <c r="B46" t="s">
-        <v>208</v>
+        <v>40</v>
       </c>
       <c r="C46" s="37" t="s">
         <v>209</v>
@@ -5181,9 +5200,9 @@
         <v>210</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="30.75">
-      <c r="A47" s="31" t="s">
-        <v>13</v>
+    <row r="47" spans="1:5" ht="29.1">
+      <c r="A47" t="s">
+        <v>36</v>
       </c>
       <c r="B47" t="s">
         <v>211</v>
@@ -5191,9 +5210,48 @@
       <c r="C47" s="37" t="s">
         <v>212</v>
       </c>
+      <c r="E47"/>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" t="s">
+        <v>213</v>
+      </c>
+      <c r="C48" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="D48" t="s">
+        <v>126</v>
+      </c>
+      <c r="E48" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" t="s">
+        <v>216</v>
+      </c>
+      <c r="C49" s="37" t="s">
+        <v>217</v>
+      </c>
+      <c r="D49" t="s">
+        <v>126</v>
+      </c>
+      <c r="E49" t="s">
+        <v>218</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E47" xr:uid="{CD15778E-9931-4B41-A419-E999FE527953}"/>
+  <autoFilter ref="A1:E49" xr:uid="{CD15778E-9931-4B41-A419-E999FE527953}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E49">
+      <sortCondition ref="A1:A49"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
@@ -5202,10 +5260,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4516AE41-49F7-4A7D-8FA3-FAD1DC5E907C}">
   <sheetPr codeName="Sheet41"/>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
@@ -5225,7 +5283,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="E1" s="25" t="s">
         <v>18</v>
@@ -5239,10 +5297,10 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="6" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="B2" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
       <c r="C2" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B2&amp;" "&amp;CHAR(10)</f>
@@ -5250,21 +5308,21 @@
 </v>
       </c>
       <c r="D2" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="E2" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="F2" t="s">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="G2" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="B3" t="s">
         <v>128</v>
@@ -5275,24 +5333,24 @@
 </v>
       </c>
       <c r="D3" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="E3" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="F3" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
       <c r="G3" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="6" t="s">
-        <v>223</v>
+        <v>229</v>
       </c>
       <c r="B4" t="s">
-        <v>211</v>
+        <v>140</v>
       </c>
       <c r="C4" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B4&amp;" "&amp;CHAR(10)</f>
@@ -5302,7 +5360,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="6" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="B5" t="s">
         <v>135</v>
@@ -5315,7 +5373,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="6" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B6" t="s">
         <v>131</v>
@@ -5328,7 +5386,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="6" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="B7" t="s">
         <v>137</v>
@@ -5336,6 +5394,19 @@
       <c r="C7" t="str">
         <f>'Data Resource Digest Submission'!$C$15&amp;B7&amp;" "&amp;CHAR(10)</f>
         <v xml:space="preserve">Xenograft 
+</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" t="str">
+        <f>'Data Resource Digest Submission'!$C$15&amp;B8&amp;" "&amp;CHAR(10)</f>
+        <v xml:space="preserve">Biospecimen 
 </v>
       </c>
     </row>
@@ -5349,8 +5420,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="31d54ef3ca738e332da14dc10991e335">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e2789f7211f2f0296d09b7bbdbdf6676" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002BAA57F805DE4D498A43031B16C0C8A1" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="23634515e2fd75be5bfad7623104c70a">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00850a8a-55a0-4f29-bb56-d3de9b9bc75c" xmlns:ns3="33e70369-3675-4c3b-99e1-030eb9633bdf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="305374924f9daf7f55b4f039a6f85780" ns2:_="" ns3:_="">
     <xsd:import namespace="00850a8a-55a0-4f29-bb56-d3de9b9bc75c"/>
     <xsd:import namespace="33e70369-3675-4c3b-99e1-030eb9633bdf"/>
     <xsd:element name="properties">
@@ -5371,6 +5442,8 @@
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
                 <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -5429,6 +5502,16 @@
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
         </xsd:sequence>
       </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="21" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="22" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="33e70369-3675-4c3b-99e1-030eb9633bdf" elementFormDefault="qualified">
@@ -5572,6 +5655,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="00850a8a-55a0-4f29-bb56-d3de9b9bc75c">
@@ -5582,23 +5674,14 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8CA60CD-2286-4C35-8489-90021763D1F5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F2AA8D1-2DD3-4347-BA28-17A66FDC41D1}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAC26B0D-F1C9-4B83-9743-12952380C0A1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{722799C8-19D7-48DA-861A-B77FE73B4586}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{722799C8-19D7-48DA-861A-B77FE73B4586}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CAC26B0D-F1C9-4B83-9743-12952380C0A1}"/>
 </file>
</xml_diff>